<commit_message>
new chain_detailsresults scneario 1 and 7
</commit_message>
<xml_diff>
--- a/Traceback_Model/Data/Results/results.xlsx
+++ b/Traceback_Model/Data/Results/results.xlsx
@@ -412,7 +412,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -425,22 +425,22 @@
         </is>
       </c>
       <c r="D2">
-        <v>5.666666627204329</v>
+        <v>0.9007217937885342</v>
       </c>
       <c r="E2">
-        <v>0.002600253262671558</v>
+        <v>0.06886383948735718</v>
       </c>
       <c r="F2">
-        <v>-19.97866136776995</v>
+        <v>-17.60655854649039</v>
       </c>
       <c r="G2">
-        <v>18.93154138288407</v>
+        <v>17.43300656077044</v>
       </c>
       <c r="H2">
-        <v>2.094239969771763</v>
+        <v>0.3471039714398998</v>
       </c>
       <c r="I2">
-        <v>0.3509470277888985</v>
+        <v>0.8406734470115096</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -450,35 +450,35 @@
     </row>
     <row r="3">
       <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chain 1_5_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chain 2</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.001000000000038916</v>
+      </c>
+      <c r="E3">
+        <v>49.99999986057535</v>
+      </c>
+      <c r="F3">
+        <v>-17.60655854649039</v>
+      </c>
+      <c r="G3">
+        <v>17.60658123503512</v>
+      </c>
+      <c r="H3">
+        <v>-4.537708944951646e-05</v>
+      </c>
+      <c r="I3">
         <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Chain 1_5_1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Chain 2</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>0.03043613394962201</v>
-      </c>
-      <c r="E3">
-        <v>0.3283477800329644</v>
-      </c>
-      <c r="F3">
-        <v>-19.97866136776995</v>
-      </c>
-      <c r="G3">
-        <v>19.97692320989285</v>
-      </c>
-      <c r="H3">
-        <v>0.003476315754198822</v>
-      </c>
-      <c r="I3">
-        <v>0.9982633518444652</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -488,35 +488,35 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chain 2_5_1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Chain 1</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.001000000000003481</v>
+      </c>
+      <c r="E4">
+        <v>49.99999784264019</v>
+      </c>
+      <c r="F4">
+        <v>-20.49413135993761</v>
+      </c>
+      <c r="G4">
+        <v>20.49415386146449</v>
+      </c>
+      <c r="H4">
+        <v>-4.500305375643165e-05</v>
+      </c>
+      <c r="I4">
         <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Chain 2_5_1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Chain 1</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>0.0128620332766471</v>
-      </c>
-      <c r="E4">
-        <v>0.8190927768978415</v>
-      </c>
-      <c r="F4">
-        <v>-19.97866136776995</v>
-      </c>
-      <c r="G4">
-        <v>19.97716380134273</v>
-      </c>
-      <c r="H4">
-        <v>0.002995132854437088</v>
-      </c>
-      <c r="I4">
-        <v>0.9985035543658263</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -539,22 +539,22 @@
         </is>
       </c>
       <c r="D5">
-        <v>6.902865856119024</v>
+        <v>0.8486166910306896</v>
       </c>
       <c r="E5">
-        <v>0.07907924617374154</v>
+        <v>0.1657004664173341</v>
       </c>
       <c r="F5">
-        <v>-19.97866136776995</v>
+        <v>-20.49413135993761</v>
       </c>
       <c r="G5">
-        <v>18.20296122500276</v>
+        <v>20.33119640499809</v>
       </c>
       <c r="H5">
-        <v>3.551400285534378</v>
+        <v>0.3258699098790458</v>
       </c>
       <c r="I5">
-        <v>0.1693648284188363</v>
+        <v>0.8496464519221111</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -594,13 +594,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>159.6836849540449</v>
+        <v>16.83176100781197</v>
       </c>
       <c r="C2">
-        <v>0.06185859259216098</v>
+        <v>0.0001876266873183097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>